<commit_message>
Added idea to spreadsheet
</commit_message>
<xml_diff>
--- a/WorkoutPlannerdata.xlsx
+++ b/WorkoutPlannerdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f310c4b36d78254d/Desktop/Github Repositories/WorkoutPlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{D6F22301-7F14-4431-A60D-62F8CA8AE2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9AF67AB-E922-4F05-9931-5A9A47032B62}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="8_{D6F22301-7F14-4431-A60D-62F8CA8AE2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29C02E5D-402A-4225-8AD7-76F9CC367D51}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F383DB04-FFA1-44A5-BDAF-8A390703A2BB}"/>
   </bookViews>
@@ -35,44 +35,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
   <si>
-    <t>Exercises</t>
-  </si>
-  <si>
-    <t>Benchpress</t>
-  </si>
-  <si>
-    <t>Squat</t>
-  </si>
-  <si>
-    <t>Deadlift</t>
-  </si>
-  <si>
     <t>PR</t>
   </si>
   <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>Week 1.1</t>
-  </si>
-  <si>
-    <t>Week 1.2</t>
-  </si>
-  <si>
-    <t>Week 2.1</t>
-  </si>
-  <si>
-    <t>Week 2.2</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -88,46 +61,94 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Push</t>
-  </si>
-  <si>
     <t xml:space="preserve">Leg </t>
   </si>
   <si>
-    <t>Pull</t>
-  </si>
-  <si>
     <t>Risk</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
-    <t>20-50</t>
-  </si>
-  <si>
-    <t>10-20.0</t>
-  </si>
-  <si>
     <t>Core</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Recent</t>
   </si>
   <si>
-    <t>Knee</t>
-  </si>
-  <si>
-    <t>Moderate</t>
-  </si>
-  <si>
-    <t>Male</t>
+    <t>benchpress</t>
+  </si>
+  <si>
+    <t>push</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>pull</t>
+  </si>
+  <si>
+    <t>deadlift</t>
+  </si>
+  <si>
+    <t>squat</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>knee</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>bob</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>rack</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>Muscle</t>
+  </si>
+  <si>
+    <t>chest</t>
+  </si>
+  <si>
+    <t>quad</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Simple version below….</t>
+  </si>
+  <si>
+    <t>XXXXXXXX</t>
+  </si>
+  <si>
+    <t>"-2  is Goal"</t>
+  </si>
+  <si>
+    <t>"-1 is PR</t>
+  </si>
+  <si>
+    <t>"0 is recent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 is first exercise etc </t>
   </si>
 </sst>
 </file>
@@ -165,7 +186,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,162 +501,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9FCEF8-4809-4741-B1EA-D07DBCF411B1}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>30</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>180</v>
+      </c>
+      <c r="I6">
+        <v>150</v>
+      </c>
+      <c r="J6">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>200</v>
+      </c>
+      <c r="I7">
+        <v>150</v>
+      </c>
+      <c r="J7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8">
+        <v>250</v>
+      </c>
+      <c r="I8">
+        <v>200</v>
+      </c>
+      <c r="J8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>-2</v>
+      </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
         <v>5</v>
       </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6">
-        <v>180</v>
-      </c>
-      <c r="G6">
-        <v>150</v>
-      </c>
-      <c r="H6">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7">
-        <v>200</v>
-      </c>
-      <c r="G7">
-        <v>150</v>
-      </c>
-      <c r="H7">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8">
-        <v>250</v>
-      </c>
-      <c r="G8">
-        <v>200</v>
-      </c>
-      <c r="H8">
-        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
notes added about current pandas syntax
</commit_message>
<xml_diff>
--- a/WorkoutPlannerdata.xlsx
+++ b/WorkoutPlannerdata.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f310c4b36d78254d/Desktop/Github Repositories/WorkoutPlanner/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_08592007B630921FD2FE31D2F8F2D3C2A4580014" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6910A79-7E13-4130-A528-82E570EA41DC}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -52,8 +58,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +122,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -162,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,9 +208,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,6 +260,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,14 +453,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -444,7 +496,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -461,7 +513,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -478,7 +530,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -495,7 +547,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -503,12 +555,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
-      </c>
-      <c r="C7">
-        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more detailed description added
</commit_message>
<xml_diff>
--- a/WorkoutPlannerdata.xlsx
+++ b/WorkoutPlannerdata.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f310c4b36d78254d/Desktop/Github Repositories/WorkoutPlanner/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_08592007B630921FD2FE31D2F8F2D3C2A4580014" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6910A79-7E13-4130-A528-82E570EA41DC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -58,8 +52,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,14 +116,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -176,7 +162,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,27 +194,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,24 +228,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,16 +403,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -496,7 +444,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -513,7 +461,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -530,7 +478,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -547,17 +495,38 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>350</v>
+      </c>
+      <c r="D6">
+        <v>450</v>
+      </c>
+      <c r="E6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
+      </c>
+      <c r="B7">
+        <v>210</v>
+      </c>
+      <c r="C7">
+        <v>360</v>
+      </c>
+      <c r="D7">
+        <v>450</v>
+      </c>
+      <c r="E7">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>